<commit_message>
added stim/ to testloop, not yet to actual exp loop xls file
</commit_message>
<xml_diff>
--- a/testTrialLoop.xlsx
+++ b/testTrialLoop.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zixuan/Documents/face_loc_Mooney/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2811755-16E7-824F-83F9-DE963DC21355}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3E58E35-F3B7-FA40-803F-8939121224C9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="23040" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,28 +31,28 @@
     <t>image</t>
   </si>
   <si>
-    <t>1.bmp</t>
-  </si>
-  <si>
-    <t>5.bmp</t>
-  </si>
-  <si>
-    <t>9.bmp</t>
-  </si>
-  <si>
-    <t>13.bmp</t>
-  </si>
-  <si>
-    <t>17.bmp</t>
-  </si>
-  <si>
-    <t>21.bmp</t>
-  </si>
-  <si>
-    <t>25.bmp</t>
-  </si>
-  <si>
-    <t>29.bmp</t>
+    <t>stim/1.bmp</t>
+  </si>
+  <si>
+    <t>stim/5.bmp</t>
+  </si>
+  <si>
+    <t>stim/9.bmp</t>
+  </si>
+  <si>
+    <t>stim/13.bmp</t>
+  </si>
+  <si>
+    <t>stim/17.bmp</t>
+  </si>
+  <si>
+    <t>stim/21.bmp</t>
+  </si>
+  <si>
+    <t>stim/25.bmp</t>
+  </si>
+  <si>
+    <t>stim/29.bmp</t>
   </si>
 </sst>
 </file>
@@ -372,7 +372,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>